<commit_message>
Do not save temporary excel files
</commit_message>
<xml_diff>
--- a/data/prezidento_rinkimai_2024.xlsx
+++ b/data/prezidento_rinkimai_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpiktas/R/rinkimai_20240512/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43769E36-6492-2140-B268-34161762FF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD819FA5-2785-9E4F-AEE9-56A1564578BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="18880" activeTab="5" xr2:uid="{AC3A57F6-202B-7B43-8D73-6AF1FDA1C625}"/>
   </bookViews>
@@ -3101,7 +3101,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update data, create report, add webpage
</commit_message>
<xml_diff>
--- a/data/prezidento_rinkimai_2024.xlsx
+++ b/data/prezidento_rinkimai_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpiktas/R/rinkimai_20240512/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275B5219-AA51-6243-A4F1-DB37B647B096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDBB1AE-FF19-B346-8AAE-55191C1B335E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="18880" activeTab="6" xr2:uid="{AC3A57F6-202B-7B43-8D73-6AF1FDA1C625}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="18880" activeTab="8" xr2:uid="{AC3A57F6-202B-7B43-8D73-6AF1FDA1C625}"/>
   </bookViews>
   <sheets>
     <sheet name="20_45" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="21_45" sheetId="5" r:id="rId5"/>
     <sheet name="22_00" sheetId="6" r:id="rId6"/>
     <sheet name="22_15" sheetId="7" r:id="rId7"/>
+    <sheet name="22_30" sheetId="8" r:id="rId8"/>
+    <sheet name="22_45" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="54">
   <si>
     <r>
       <t>Apylinkių skaičius - </t>
@@ -1563,6 +1565,428 @@
         <family val="2"/>
       </rPr>
       <t>99,21</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>%).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Apylinkių skaičius - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1895</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (duomenys iš 1008 apylinkių)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Savivaldybių skaičius - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>60</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(duomenys iš 57 savivaldybių)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> rinkėjų sąraše įrašyta rinkėjų - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>542720</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, rinkimuose dalyvavo - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>302019</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>55,65</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>%),</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> negaliojančių biuletenių - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2399</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0,79</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>%), galiojančių biuletenių - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>299620</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>99,21</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>%).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Apylinkių skaičius - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1895</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (duomenys iš 1090 apylinkių)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Savivaldybių skaičius - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>60</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(duomenys iš 58 savivaldybių)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> rinkėjų sąraše įrašyta rinkėjų - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>632563</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, rinkimuose dalyvavo - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>351977</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>55,64</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>%),</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> negaliojančių biuletenių - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2850</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0,81</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>%), galiojančių biuletenių - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>349127</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>99,19</t>
     </r>
     <r>
       <rPr>
@@ -3575,9 +3999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EC1CD5-1B54-5B48-8C82-1CC878B15DC3}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -3832,4 +4254,530 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E77BAC-B9B3-8644-9AFB-A2EDEB6ED66B}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1">
+        <v>112172</v>
+      </c>
+      <c r="C11" s="1">
+        <v>37728</v>
+      </c>
+      <c r="D11" s="1">
+        <v>149900</v>
+      </c>
+      <c r="E11" s="1">
+        <v>50.03</v>
+      </c>
+      <c r="F11" s="1">
+        <v>49.63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1">
+        <v>33753</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5483</v>
+      </c>
+      <c r="D12" s="1">
+        <v>39236</v>
+      </c>
+      <c r="E12" s="1">
+        <v>13.1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>12.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1">
+        <v>29591</v>
+      </c>
+      <c r="C13" s="1">
+        <v>6569</v>
+      </c>
+      <c r="D13" s="1">
+        <v>36160</v>
+      </c>
+      <c r="E13" s="1">
+        <v>12.07</v>
+      </c>
+      <c r="F13" s="1">
+        <v>11.97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <v>25317</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10581</v>
+      </c>
+      <c r="D14" s="1">
+        <v>35898</v>
+      </c>
+      <c r="E14" s="1">
+        <v>11.98</v>
+      </c>
+      <c r="F14" s="1">
+        <v>11.89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1">
+        <v>18465</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3636</v>
+      </c>
+      <c r="D15" s="1">
+        <v>22101</v>
+      </c>
+      <c r="E15" s="1">
+        <v>7.38</v>
+      </c>
+      <c r="F15" s="1">
+        <v>7.32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1">
+        <v>5412</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2071</v>
+      </c>
+      <c r="D16" s="1">
+        <v>7483</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1">
+        <v>3603</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1360</v>
+      </c>
+      <c r="D17" s="1">
+        <v>4963</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1.66</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2819</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1060</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3879</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1.29</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="3">
+        <v>231132</v>
+      </c>
+      <c r="C19" s="3">
+        <v>68488</v>
+      </c>
+      <c r="D19" s="3">
+        <v>299620</v>
+      </c>
+      <c r="E19" s="3">
+        <v>100</v>
+      </c>
+      <c r="F19" s="3">
+        <v>99.21</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A11" r:id="rId1" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435326.html" xr:uid="{3364F719-54C4-4648-8393-6F46CBCDBD2B}"/>
+    <hyperlink ref="A12" r:id="rId2" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435327.html" xr:uid="{DDF2E22F-FAC9-9348-829F-DAEC18DE59D4}"/>
+    <hyperlink ref="A13" r:id="rId3" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435334.html" xr:uid="{3DEE5ECC-973C-E940-8A06-530B668DB95E}"/>
+    <hyperlink ref="A14" r:id="rId4" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435331.html" xr:uid="{AA634C6A-F905-1A43-9615-84D2B446A377}"/>
+    <hyperlink ref="A15" r:id="rId5" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435325.html" xr:uid="{7BC4F0A4-A8E5-B04F-8841-8810C3377181}"/>
+    <hyperlink ref="A16" r:id="rId6" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435333.html" xr:uid="{912575AB-0C57-D041-A13B-2FFA0891AFDA}"/>
+    <hyperlink ref="A17" r:id="rId7" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435329.html" xr:uid="{42816C31-E84F-AA49-A281-DBE684B102DB}"/>
+    <hyperlink ref="A18" r:id="rId8" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435328.html" xr:uid="{6D61107D-83FE-7A48-BFAC-539A42E63375}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A75C3FD8-2E99-5945-B1F1-8894FA218F50}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1">
+        <v>130713</v>
+      </c>
+      <c r="C11" s="1">
+        <v>43103</v>
+      </c>
+      <c r="D11" s="1">
+        <v>173816</v>
+      </c>
+      <c r="E11" s="1">
+        <v>49.79</v>
+      </c>
+      <c r="F11" s="1">
+        <v>49.38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1">
+        <v>38622</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6280</v>
+      </c>
+      <c r="D12" s="1">
+        <v>44902</v>
+      </c>
+      <c r="E12" s="1">
+        <v>12.86</v>
+      </c>
+      <c r="F12" s="1">
+        <v>12.76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1">
+        <v>30542</v>
+      </c>
+      <c r="C13" s="1">
+        <v>12359</v>
+      </c>
+      <c r="D13" s="1">
+        <v>42901</v>
+      </c>
+      <c r="E13" s="1">
+        <v>12.29</v>
+      </c>
+      <c r="F13" s="1">
+        <v>12.19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>34818</v>
+      </c>
+      <c r="C14" s="1">
+        <v>7684</v>
+      </c>
+      <c r="D14" s="1">
+        <v>42502</v>
+      </c>
+      <c r="E14" s="1">
+        <v>12.17</v>
+      </c>
+      <c r="F14" s="1">
+        <v>12.08</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1">
+        <v>21773</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4133</v>
+      </c>
+      <c r="D15" s="1">
+        <v>25906</v>
+      </c>
+      <c r="E15" s="1">
+        <v>7.42</v>
+      </c>
+      <c r="F15" s="1">
+        <v>7.36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1">
+        <v>6457</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2418</v>
+      </c>
+      <c r="D16" s="1">
+        <v>8875</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2.54</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1">
+        <v>4153</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1542</v>
+      </c>
+      <c r="D17" s="1">
+        <v>5695</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1.63</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3304</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1226</v>
+      </c>
+      <c r="D18" s="1">
+        <v>4530</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="3">
+        <v>270382</v>
+      </c>
+      <c r="C19" s="3">
+        <v>78745</v>
+      </c>
+      <c r="D19" s="3">
+        <v>349127</v>
+      </c>
+      <c r="E19" s="3">
+        <v>100</v>
+      </c>
+      <c r="F19" s="3">
+        <v>99.19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A11" r:id="rId1" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435326.html" xr:uid="{7FCF0334-CD3D-2C45-974E-5675F41BBA42}"/>
+    <hyperlink ref="A12" r:id="rId2" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435327.html" xr:uid="{F1BD83E5-E34F-3248-B7F5-D0287454929D}"/>
+    <hyperlink ref="A13" r:id="rId3" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435331.html" xr:uid="{9D8B5894-BA70-6845-8A9B-82EFD0AC8F68}"/>
+    <hyperlink ref="A14" r:id="rId4" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435334.html" xr:uid="{E1935A9D-A0B2-3346-AE7D-14A240BD43EF}"/>
+    <hyperlink ref="A15" r:id="rId5" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435325.html" xr:uid="{873D142E-140F-B847-ACB1-D2A7EB497DAC}"/>
+    <hyperlink ref="A16" r:id="rId6" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435333.html" xr:uid="{80891E70-85C3-D54D-BBD7-A524AF7389E7}"/>
+    <hyperlink ref="A17" r:id="rId7" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435329.html" xr:uid="{8A194E98-861F-2646-8469-2353A9D39BCA}"/>
+    <hyperlink ref="A18" r:id="rId8" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435328.html" xr:uid="{D0130C03-1C62-734B-9F58-440E8039AE63}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update colours and data
</commit_message>
<xml_diff>
--- a/data/prezidento_rinkimai_2024.xlsx
+++ b/data/prezidento_rinkimai_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpiktas/R/rinkimai_20240512/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDBB1AE-FF19-B346-8AAE-55191C1B335E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31689A87-274A-9B43-BAF0-185DB890ED33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="18880" activeTab="8" xr2:uid="{AC3A57F6-202B-7B43-8D73-6AF1FDA1C625}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="18880" activeTab="9" xr2:uid="{AC3A57F6-202B-7B43-8D73-6AF1FDA1C625}"/>
   </bookViews>
   <sheets>
     <sheet name="20_45" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="22_15" sheetId="7" r:id="rId7"/>
     <sheet name="22_30" sheetId="8" r:id="rId8"/>
     <sheet name="22_45" sheetId="9" r:id="rId9"/>
+    <sheet name="23_00" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="57">
   <si>
     <r>
       <t>Apylinkių skaičius - </t>
@@ -1987,6 +1988,183 @@
         <family val="2"/>
       </rPr>
       <t>99,19</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>%).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Apylinkių skaičius - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1895</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (duomenys iš 1172 apylinkių)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> rinkėjų sąraše įrašyta rinkėjų - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>752758</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, rinkimuose dalyvavo - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>420889</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>55,91</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>%),</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> negaliojančių biuletenių - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3444</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0,82</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>%), galiojančių biuletenių - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>417445</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>99,18</t>
     </r>
     <r>
       <rPr>
@@ -2673,6 +2851,269 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85804DFE-075E-6D41-AFD0-EC62D8881128}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1">
+        <v>155624</v>
+      </c>
+      <c r="C11" s="1">
+        <v>49605</v>
+      </c>
+      <c r="D11" s="1">
+        <v>205229</v>
+      </c>
+      <c r="E11" s="1">
+        <v>49.16</v>
+      </c>
+      <c r="F11" s="1">
+        <v>48.76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1">
+        <v>38245</v>
+      </c>
+      <c r="C12" s="1">
+        <v>15414</v>
+      </c>
+      <c r="D12" s="1">
+        <v>53659</v>
+      </c>
+      <c r="E12" s="1">
+        <v>12.85</v>
+      </c>
+      <c r="F12" s="1">
+        <v>12.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44999</v>
+      </c>
+      <c r="C13" s="1">
+        <v>7349</v>
+      </c>
+      <c r="D13" s="1">
+        <v>52348</v>
+      </c>
+      <c r="E13" s="1">
+        <v>12.54</v>
+      </c>
+      <c r="F13" s="1">
+        <v>12.44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>42023</v>
+      </c>
+      <c r="C14" s="1">
+        <v>9051</v>
+      </c>
+      <c r="D14" s="1">
+        <v>51074</v>
+      </c>
+      <c r="E14" s="1">
+        <v>12.23</v>
+      </c>
+      <c r="F14" s="1">
+        <v>12.13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1">
+        <v>27006</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4968</v>
+      </c>
+      <c r="D15" s="1">
+        <v>31974</v>
+      </c>
+      <c r="E15" s="1">
+        <v>7.66</v>
+      </c>
+      <c r="F15" s="1">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1">
+        <v>7882</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3047</v>
+      </c>
+      <c r="D16" s="1">
+        <v>10929</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2.62</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1">
+        <v>4994</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1845</v>
+      </c>
+      <c r="D17" s="1">
+        <v>6839</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1.64</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3910</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1483</v>
+      </c>
+      <c r="D18" s="1">
+        <v>5393</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1.29</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="3">
+        <v>324683</v>
+      </c>
+      <c r="C19" s="3">
+        <v>92762</v>
+      </c>
+      <c r="D19" s="3">
+        <v>417445</v>
+      </c>
+      <c r="E19" s="3">
+        <v>100</v>
+      </c>
+      <c r="F19" s="3">
+        <v>99.18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A11" r:id="rId1" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435326.html" xr:uid="{8FCA261B-5200-EF48-A0BF-0C4A41BF8CC4}"/>
+    <hyperlink ref="A12" r:id="rId2" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435331.html" xr:uid="{513E0344-1162-334B-80ED-ACDC1467D989}"/>
+    <hyperlink ref="A13" r:id="rId3" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435327.html" xr:uid="{387284F9-9AAB-0740-BB19-B0D9E31F930F}"/>
+    <hyperlink ref="A14" r:id="rId4" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435334.html" xr:uid="{A43E0398-F2A3-D44A-A70C-170EF9B2A19F}"/>
+    <hyperlink ref="A15" r:id="rId5" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435325.html" xr:uid="{99C9F9E9-B093-ED4C-9B6D-6BAE75687465}"/>
+    <hyperlink ref="A16" r:id="rId6" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435333.html" xr:uid="{D09CEE8E-F64D-6542-9A2D-DEA3F3469EE6}"/>
+    <hyperlink ref="A17" r:id="rId7" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435329.html" xr:uid="{81575037-DE9F-A84B-9A0F-2841EDFAE3F7}"/>
+    <hyperlink ref="A18" r:id="rId8" display="https://rezultatai.vrk.lt/?srcUrl=/rinkimai/1504/1/2070/rezultatai/lt/rezultataiPreKandBalsLietuvoje_rkndId-2435328.html" xr:uid="{18FD49CE-68FD-B243-80C5-9BF8FE7C4B50}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2503F5-8769-EF41-BADD-9449FFCE94FE}">
   <dimension ref="A1:F19"/>
@@ -4523,7 +4964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A75C3FD8-2E99-5945-B1F1-8894FA218F50}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>